<commit_message>
des pas sur la neige figures
</commit_message>
<xml_diff>
--- a/analysis/ondine/ondine.xlsx
+++ b/analysis/ondine/ondine.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
   <si>
     <t>A</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Eb augumented triad(derived from 19-20)</t>
   </si>
   <si>
-    <t>A-Eb tritone, 2nd c.</t>
-  </si>
-  <si>
     <t>Eb lydian: chromatic transformation of the whole tone elements of the D lydian(m 26)</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>Pattern clearly recognizable as in 30-31</t>
   </si>
   <si>
-    <t>octatonic scale 2, whole tone 1</t>
-  </si>
-  <si>
     <t>shades in 4th c</t>
   </si>
   <si>
@@ -261,9 +255,6 @@
     <t>Octatonic 0 motif O</t>
   </si>
   <si>
-    <t xml:space="preserve">octatonic 1 </t>
-  </si>
-  <si>
     <t>F#-C#-G left, tritone</t>
   </si>
   <si>
@@ -279,9 +270,6 @@
     <t>D#(Eb)-F#</t>
   </si>
   <si>
-    <t>octatonic 1</t>
-  </si>
-  <si>
     <t>oct 0 - oct1 fragments alternation</t>
   </si>
   <si>
@@ -336,13 +324,34 @@
     <t>5th more vivid</t>
   </si>
   <si>
-    <t>3rd c.vivid</t>
-  </si>
-  <si>
     <t>of the whole tone scale 0</t>
   </si>
   <si>
     <t>6th whole tone 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3rd c.vivid, no </t>
+  </si>
+  <si>
+    <t>fusion of D triad and F# triad D F# A# augumented</t>
+  </si>
+  <si>
+    <t>augumented triad on F? 7maj?</t>
+  </si>
+  <si>
+    <t>Tritone C#-G</t>
+  </si>
+  <si>
+    <t>A-Eb tritone, 2nd c., augumented triads 3rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> whole tone 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">octatonic 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -716,15 +725,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>96240</xdr:rowOff>
+      <xdr:colOff>73269</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>37625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>693590</xdr:colOff>
+      <xdr:colOff>766859</xdr:colOff>
       <xdr:row>147</xdr:row>
-      <xdr:rowOff>53760</xdr:rowOff>
+      <xdr:rowOff>170991</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -747,8 +756,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="20213040"/>
-          <a:ext cx="7553348" cy="6541200"/>
+          <a:off x="73269" y="19732394"/>
+          <a:ext cx="7551590" cy="6287982"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1382,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1396,7 +1405,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1560,7 +1569,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="10"/>
@@ -1623,7 +1632,7 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -1686,7 +1695,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1782,7 +1791,9 @@
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -1842,7 +1853,9 @@
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="D14" s="9" t="s">
         <v>27</v>
       </c>
@@ -1990,7 +2003,7 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="s">
@@ -2029,7 +2042,7 @@
         <v>45</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9" t="s">
@@ -2053,7 +2066,7 @@
       <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
       <c r="S18" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="1"/>
@@ -2088,7 +2101,7 @@
       <c r="Q19" s="14"/>
       <c r="R19" s="14"/>
       <c r="S19" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="T19" s="15"/>
       <c r="U19" s="4"/>
@@ -2337,7 +2350,7 @@
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N26" s="10"/>
       <c r="O26" s="1"/>
@@ -2368,7 +2381,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -2403,7 +2416,7 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
@@ -2434,7 +2447,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -2465,13 +2478,13 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N30" s="10"/>
       <c r="O30" s="1"/>
@@ -2498,7 +2511,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
@@ -2533,7 +2546,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2566,7 +2579,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2599,7 +2612,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
@@ -2699,19 +2712,19 @@
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N36" s="9"/>
       <c r="O36" s="20" t="s">
@@ -2734,23 +2747,23 @@
       <c r="A37" s="8"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N37" s="9"/>
       <c r="O37" s="9" t="s">
@@ -2759,7 +2772,7 @@
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
       <c r="R37" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S37" s="9"/>
       <c r="T37" s="10"/>
@@ -2775,7 +2788,7 @@
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -2787,7 +2800,7 @@
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
@@ -2808,11 +2821,11 @@
       <c r="A39" s="8"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
@@ -2841,13 +2854,13 @@
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
@@ -2855,7 +2868,7 @@
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
@@ -2881,14 +2894,14 @@
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
@@ -3065,7 +3078,7 @@
         <v>20</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
@@ -3094,14 +3107,16 @@
       <c r="A47" s="8"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G47" s="9"/>
+      <c r="G47" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
@@ -3159,7 +3174,7 @@
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
@@ -3168,7 +3183,7 @@
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N49" s="9"/>
       <c r="O49" s="10"/>
@@ -3193,7 +3208,7 @@
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
@@ -3224,7 +3239,7 @@
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="21"/>

</xml_diff>